<commit_message>
XLS File path changes
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite NI Director Cease and recommence201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite NI Director Cease and recommence201718.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="90" windowWidth="14340" windowHeight="4455" firstSheet="22" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="90" windowWidth="14340" windowHeight="4455" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="90">
   <si>
     <t>TC</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>All</t>
-  </si>
-  <si>
-    <t>F:\\Automation NI Reports\\HMRCTestData\\Payroll Tax Test Report 201718\\201718 Payroll NI Director's calculation Test result.xlsx</t>
   </si>
   <si>
     <t>TestReportWorksheetNo</t>
@@ -321,7 +318,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,7 +424,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -762,7 +759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -807,7 +804,7 @@
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>13</v>
@@ -821,7 +818,7 @@
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>13</v>
@@ -835,7 +832,7 @@
     </row>
     <row r="5" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -849,7 +846,7 @@
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
@@ -863,10 +860,10 @@
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
@@ -877,7 +874,7 @@
     </row>
     <row r="8" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -891,7 +888,7 @@
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>13</v>
@@ -905,10 +902,10 @@
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
@@ -919,7 +916,7 @@
     </row>
     <row r="11" spans="1:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
@@ -933,7 +930,7 @@
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>13</v>
@@ -947,10 +944,10 @@
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
@@ -961,7 +958,7 @@
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -975,7 +972,7 @@
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>13</v>
@@ -989,10 +986,10 @@
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
@@ -1003,7 +1000,7 @@
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -1017,7 +1014,7 @@
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>13</v>
@@ -1031,10 +1028,10 @@
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
@@ -1045,7 +1042,7 @@
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
@@ -1059,7 +1056,7 @@
     </row>
     <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>13</v>
@@ -1073,10 +1070,10 @@
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1087,7 +1084,7 @@
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>11</v>
@@ -1101,7 +1098,7 @@
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>13</v>
@@ -1115,10 +1112,10 @@
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>4</v>
@@ -1129,7 +1126,7 @@
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
@@ -1148,11 +1145,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1199,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -1219,28 +1216,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -1252,20 +1249,20 @@
         <v>4</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1312,16 +1309,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>0.12</v>
@@ -1340,11 +1337,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,28 +1405,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -1440,18 +1437,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,7 +1499,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -1519,28 +1516,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -1554,15 +1551,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1611,16 +1608,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>30000</v>
@@ -1639,11 +1636,11 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,28 +1703,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -1738,18 +1735,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,7 +1796,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -1816,7 +1813,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -1825,19 +1822,19 @@
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -1851,16 +1848,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" display="https://eu2.salesforce.com/a2Qb0000000E8HTEA0" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink ref="C2" r:id="rId3" display="https://eu2.salesforce.com/a2Qb0000000E8HTEA0"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1906,16 +1903,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -1934,11 +1931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,28 +1998,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -2033,18 +2030,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2092,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -2112,28 +2109,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -2147,15 +2144,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2205,16 +2202,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>97968.48</v>
@@ -2234,7 +2231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2282,16 +2279,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -2310,11 +2307,11 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,28 +2374,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -2409,18 +2406,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,7 +2467,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -2487,7 +2484,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -2496,19 +2493,19 @@
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -2522,16 +2519,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" display="https://eu2.salesforce.com/a2Qb0000000E8HTEA0" xr:uid="{00000000-0004-0000-1500-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink ref="C2" r:id="rId3" display="https://eu2.salesforce.com/a2Qb0000000E8HTEA0"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2579,16 +2576,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>546000</v>
@@ -2607,11 +2604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,28 +2671,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -2706,17 +2703,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -2767,7 +2764,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -2784,28 +2781,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -2819,18 +2816,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,10 +2890,10 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
@@ -2905,13 +2902,13 @@
         <v>30</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>31</v>
@@ -2925,18 +2922,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2986,7 +2983,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -3003,10 +3000,10 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
@@ -3015,16 +3012,16 @@
         <v>30</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -3038,14 +3035,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3093,16 +3090,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>0.12</v>
@@ -3122,11 +3119,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3189,28 +3186,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -3221,18 +3218,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3283,7 +3280,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>2</v>
@@ -3300,28 +3297,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -3335,14 +3332,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3391,16 +3388,16 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6">
         <v>0.6</v>
@@ -3420,11 +3417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3487,28 +3484,28 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>32</v>
@@ -3519,7 +3516,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>